<commit_message>
Adding API Postman Design Link on readme file
</commit_message>
<xml_diff>
--- a/00-project-designs/Excel/database-schemaxlsx.xlsx
+++ b/00-project-designs/Excel/database-schemaxlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\09-Projects\Tasks-for-companies\SLA-System\00-project-designs\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C6D467-4D0B-4DC2-9D14-6E6B54346512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147B61AC-D71D-43A9-B4CE-3284551A63B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1344" windowWidth="23256" windowHeight="12456" xr2:uid="{2B7ABF8D-7985-4773-A7F1-66F8C8F7F7B2}"/>
+    <workbookView xWindow="13005" yWindow="3825" windowWidth="17280" windowHeight="8880" xr2:uid="{2B7ABF8D-7985-4773-A7F1-66F8C8F7F7B2}"/>
   </bookViews>
   <sheets>
     <sheet name="database-schema" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Request</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>request_status</t>
   </si>
 </sst>
 </file>
@@ -618,21 +621,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="13" width="13.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="14" width="13.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
@@ -642,7 +645,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -650,7 +653,7 @@
       <c r="J2" s="10"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -668,7 +671,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -700,12 +703,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -723,7 +726,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>1</v>
       </c>
@@ -752,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11" s="12" t="s">
         <v>0</v>
       </c>
@@ -765,8 +768,9 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
@@ -776,36 +780,39 @@
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="M12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>6</v>
+      <c r="N12" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="F1:K2"/>
-    <mergeCell ref="D11:M11"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="D7:I7"/>
+    <mergeCell ref="D11:N11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finishing Request Domain Model
</commit_message>
<xml_diff>
--- a/00-project-designs/Excel/database-schemaxlsx.xlsx
+++ b/00-project-designs/Excel/database-schemaxlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\09-Projects\Tasks-for-companies\SLA-System\00-project-designs\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147B61AC-D71D-43A9-B4CE-3284551A63B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96515B0-F068-4F80-9C88-4C706F2BE695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13005" yWindow="3825" windowWidth="17280" windowHeight="8880" xr2:uid="{2B7ABF8D-7985-4773-A7F1-66F8C8F7F7B2}"/>
+    <workbookView xWindow="-23148" yWindow="1344" windowWidth="23256" windowHeight="12456" xr2:uid="{2B7ABF8D-7985-4773-A7F1-66F8C8F7F7B2}"/>
   </bookViews>
   <sheets>
     <sheet name="database-schema" sheetId="1" r:id="rId1"/>
@@ -623,8 +623,8 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,12 +807,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D11:N11"/>
     <mergeCell ref="F1:K2"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D11:N11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>